<commit_message>
for prime center, remove duplicate lines and stacking completely works
</commit_message>
<xml_diff>
--- a/documents/paklijst.xlsx
+++ b/documents/paklijst.xlsx
@@ -1057,22 +1057,21 @@
   </sheetPr>
   <dimension ref="1:74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="42.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="13.5"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3222,6 +3221,8 @@
       <c r="I6" s="17" t="s">
         <v>18</v>
       </c>
+      <c r="J6" s="0"/>
+      <c r="K6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
@@ -3251,6 +3252,8 @@
       <c r="I7" s="17" t="s">
         <v>21</v>
       </c>
+      <c r="J7" s="0"/>
+      <c r="K7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
@@ -3280,6 +3283,8 @@
       <c r="I8" s="17" t="s">
         <v>24</v>
       </c>
+      <c r="J8" s="0"/>
+      <c r="K8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="16" t="s">
@@ -3309,6 +3314,8 @@
       <c r="I9" s="17" t="s">
         <v>28</v>
       </c>
+      <c r="J9" s="0"/>
+      <c r="K9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
@@ -3338,6 +3345,8 @@
       <c r="I10" s="17" t="s">
         <v>31</v>
       </c>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
@@ -3367,6 +3376,8 @@
       <c r="I11" s="17" t="s">
         <v>36</v>
       </c>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
@@ -3396,6 +3407,8 @@
       <c r="I12" s="17" t="s">
         <v>38</v>
       </c>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="16" t="s">
@@ -3425,6 +3438,8 @@
       <c r="I13" s="17" t="s">
         <v>42</v>
       </c>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
@@ -3454,6 +3469,8 @@
       <c r="I14" s="17" t="s">
         <v>45</v>
       </c>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
@@ -3483,6 +3500,8 @@
       <c r="I15" s="17" t="s">
         <v>48</v>
       </c>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
@@ -3512,6 +3531,8 @@
       <c r="I16" s="17" t="s">
         <v>51</v>
       </c>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="16" t="s">
@@ -3541,6 +3562,8 @@
       <c r="I17" s="17" t="s">
         <v>54</v>
       </c>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
@@ -3570,6 +3593,8 @@
       <c r="I18" s="17" t="s">
         <v>38</v>
       </c>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
@@ -3599,6 +3624,8 @@
       <c r="I19" s="17" t="s">
         <v>58</v>
       </c>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
@@ -3628,6 +3655,8 @@
       <c r="I20" s="17" t="s">
         <v>62</v>
       </c>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
@@ -3657,6 +3686,8 @@
       <c r="I21" s="17" t="s">
         <v>66</v>
       </c>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
@@ -3686,6 +3717,8 @@
       <c r="I22" s="17" t="s">
         <v>69</v>
       </c>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
@@ -3715,6 +3748,8 @@
       <c r="I23" s="17" t="s">
         <v>72</v>
       </c>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
@@ -3744,6 +3779,8 @@
       <c r="I24" s="17" t="s">
         <v>75</v>
       </c>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
@@ -3773,6 +3810,8 @@
       <c r="I25" s="17" t="s">
         <v>78</v>
       </c>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
@@ -3802,6 +3841,8 @@
       <c r="I26" s="17" t="s">
         <v>81</v>
       </c>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
@@ -3831,6 +3872,8 @@
       <c r="I27" s="17" t="s">
         <v>84</v>
       </c>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
@@ -3860,6 +3903,8 @@
       <c r="I28" s="17" t="s">
         <v>89</v>
       </c>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
@@ -3889,6 +3934,8 @@
       <c r="I29" s="17" t="s">
         <v>89</v>
       </c>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
@@ -3918,6 +3965,8 @@
       <c r="I30" s="17" t="s">
         <v>95</v>
       </c>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">

</xml_diff>